<commit_message>
Fourth Commit, Redoing functions
</commit_message>
<xml_diff>
--- a/Street Data_BaDinh.xlsx
+++ b/Street Data_BaDinh.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Coding\VSC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADMIN\Documents\GitHub\Street-Data-New\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C29BEC87-A4C6-4FCA-B9D0-67D30578E2DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D87A1F85-2474-4025-8341-CD6AD3B525D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3375" yWindow="3975" windowWidth="21600" windowHeight="11835" xr2:uid="{CA5F727D-DDF9-458F-9625-B8586C5DDF4C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{CA5F727D-DDF9-458F-9625-B8586C5DDF4C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2018,18 +2018,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{930306BC-B5F1-44CA-8AB8-4B085D6FDCD3}">
   <dimension ref="A1:J399"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B294" workbookViewId="0">
-      <selection activeCell="L310" sqref="L310"/>
+    <sheetView tabSelected="1" topLeftCell="B67" workbookViewId="0">
+      <selection activeCell="H82" sqref="H82:I82"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="24.85546875" customWidth="1"/>
-    <col min="8" max="8" width="11.42578125" customWidth="1"/>
-    <col min="9" max="9" width="10.5703125" customWidth="1"/>
+    <col min="4" max="4" width="24.88671875" customWidth="1"/>
+    <col min="8" max="8" width="11.44140625" customWidth="1"/>
+    <col min="9" max="9" width="10.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2061,7 +2061,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -2089,7 +2089,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -2117,7 +2117,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -2145,7 +2145,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -2173,7 +2173,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -2201,7 +2201,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>22</v>
       </c>
@@ -2229,7 +2229,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -2257,7 +2257,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>27</v>
       </c>
@@ -2285,7 +2285,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>29</v>
       </c>
@@ -2313,7 +2313,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>31</v>
       </c>
@@ -2341,7 +2341,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>35</v>
       </c>
@@ -2369,7 +2369,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>37</v>
       </c>
@@ -2397,7 +2397,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>40</v>
       </c>
@@ -2427,7 +2427,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>43</v>
       </c>
@@ -2455,7 +2455,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>46</v>
       </c>
@@ -2483,7 +2483,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>48</v>
       </c>
@@ -2511,7 +2511,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>50</v>
       </c>
@@ -2541,7 +2541,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>53</v>
       </c>
@@ -2571,7 +2571,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>55</v>
       </c>
@@ -2599,7 +2599,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>57</v>
       </c>
@@ -2627,7 +2627,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>59</v>
       </c>
@@ -2655,7 +2655,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
         <v>62</v>
       </c>
@@ -2683,7 +2683,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
         <v>65</v>
       </c>
@@ -2711,7 +2711,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
         <v>67</v>
       </c>
@@ -2739,7 +2739,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
         <v>68</v>
       </c>
@@ -2769,7 +2769,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>71</v>
       </c>
@@ -2801,7 +2801,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>74</v>
       </c>
@@ -2829,7 +2829,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>75</v>
       </c>
@@ -2857,7 +2857,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>77</v>
       </c>
@@ -2887,7 +2887,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>79</v>
       </c>
@@ -2915,7 +2915,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>80</v>
       </c>
@@ -2943,7 +2943,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>82</v>
       </c>
@@ -2971,7 +2971,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>84</v>
       </c>
@@ -3003,7 +3003,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>85</v>
       </c>
@@ -3033,7 +3033,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>89</v>
       </c>
@@ -3061,7 +3061,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
         <v>90</v>
       </c>
@@ -3089,7 +3089,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
         <v>91</v>
       </c>
@@ -3117,7 +3117,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
         <v>92</v>
       </c>
@@ -3145,7 +3145,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
         <v>94</v>
       </c>
@@ -3175,7 +3175,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>96</v>
       </c>
@@ -3203,7 +3203,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>98</v>
       </c>
@@ -3231,7 +3231,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="s">
         <v>99</v>
       </c>
@@ -3261,7 +3261,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>101</v>
       </c>
@@ -3289,7 +3289,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>103</v>
       </c>
@@ -3319,7 +3319,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A46" s="3" t="s">
         <v>105</v>
       </c>
@@ -3347,7 +3347,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A47" s="3" t="s">
         <v>107</v>
       </c>
@@ -3375,7 +3375,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>109</v>
       </c>
@@ -3403,7 +3403,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>110</v>
       </c>
@@ -3431,7 +3431,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>112</v>
       </c>
@@ -3459,7 +3459,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>113</v>
       </c>
@@ -3489,7 +3489,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>116</v>
       </c>
@@ -3517,7 +3517,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>117</v>
       </c>
@@ -3545,7 +3545,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>118</v>
       </c>
@@ -3573,7 +3573,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A55" s="3" t="s">
         <v>120</v>
       </c>
@@ -3601,7 +3601,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A56" s="3" t="s">
         <v>123</v>
       </c>
@@ -3629,7 +3629,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>124</v>
       </c>
@@ -3657,7 +3657,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>125</v>
       </c>
@@ -3685,7 +3685,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>127</v>
       </c>
@@ -3713,7 +3713,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>128</v>
       </c>
@@ -3741,7 +3741,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>129</v>
       </c>
@@ -3769,7 +3769,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>130</v>
       </c>
@@ -3797,7 +3797,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>131</v>
       </c>
@@ -3825,7 +3825,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>132</v>
       </c>
@@ -3857,7 +3857,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>133</v>
       </c>
@@ -3885,7 +3885,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>134</v>
       </c>
@@ -3913,7 +3913,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>135</v>
       </c>
@@ -3941,7 +3941,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>201</v>
       </c>
@@ -3969,7 +3969,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A69" s="3" t="s">
         <v>137</v>
       </c>
@@ -3997,7 +3997,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>139</v>
       </c>
@@ -4025,7 +4025,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>141</v>
       </c>
@@ -4053,7 +4053,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>142</v>
       </c>
@@ -4081,7 +4081,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A73" s="3" t="s">
         <v>144</v>
       </c>
@@ -4109,7 +4109,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A74" s="3" t="s">
         <v>145</v>
       </c>
@@ -4137,7 +4137,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>146</v>
       </c>
@@ -4167,7 +4167,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>147</v>
       </c>
@@ -4186,16 +4186,16 @@
       <c r="F76" s="1"/>
       <c r="G76" s="1"/>
       <c r="H76" s="1">
-        <v>21.034973000000001</v>
+        <v>21.034687000000002</v>
       </c>
       <c r="I76" s="1">
-        <v>105.823891</v>
+        <v>105.827152</v>
       </c>
       <c r="J76" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>149</v>
       </c>
@@ -4223,7 +4223,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>151</v>
       </c>
@@ -4251,7 +4251,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>152</v>
       </c>
@@ -4279,7 +4279,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>154</v>
       </c>
@@ -4307,7 +4307,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A81" s="3" t="s">
         <v>155</v>
       </c>
@@ -4335,7 +4335,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>156</v>
       </c>
@@ -4354,16 +4354,16 @@
       <c r="F82" s="1"/>
       <c r="G82" s="1"/>
       <c r="H82" s="1">
-        <v>21.034973000000001</v>
+        <v>21.034687000000002</v>
       </c>
       <c r="I82" s="1">
-        <v>105.823891</v>
+        <v>105.827152</v>
       </c>
       <c r="J82" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>157</v>
       </c>
@@ -4391,7 +4391,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>158</v>
       </c>
@@ -4423,7 +4423,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>161</v>
       </c>
@@ -4453,7 +4453,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>162</v>
       </c>
@@ -4481,7 +4481,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>164</v>
       </c>
@@ -4509,7 +4509,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>166</v>
       </c>
@@ -4537,7 +4537,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>168</v>
       </c>
@@ -4565,7 +4565,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>169</v>
       </c>
@@ -4597,7 +4597,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>170</v>
       </c>
@@ -4625,7 +4625,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>171</v>
       </c>
@@ -4653,7 +4653,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>174</v>
       </c>
@@ -4681,7 +4681,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>175</v>
       </c>
@@ -4709,7 +4709,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>176</v>
       </c>
@@ -4737,7 +4737,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>177</v>
       </c>
@@ -4765,7 +4765,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>178</v>
       </c>
@@ -4793,7 +4793,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>179</v>
       </c>
@@ -4821,7 +4821,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>180</v>
       </c>
@@ -4849,7 +4849,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>182</v>
       </c>
@@ -4879,7 +4879,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>184</v>
       </c>
@@ -4907,7 +4907,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>186</v>
       </c>
@@ -4935,7 +4935,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>188</v>
       </c>
@@ -4963,7 +4963,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>190</v>
       </c>
@@ -4993,7 +4993,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>192</v>
       </c>
@@ -5023,7 +5023,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>193</v>
       </c>
@@ -5051,7 +5051,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>194</v>
       </c>
@@ -5079,7 +5079,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>195</v>
       </c>
@@ -5109,7 +5109,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>197</v>
       </c>
@@ -5139,7 +5139,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>198</v>
       </c>
@@ -5167,7 +5167,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>199</v>
       </c>
@@ -5195,7 +5195,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>200</v>
       </c>
@@ -5223,7 +5223,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>201</v>
       </c>
@@ -5251,7 +5251,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>202</v>
       </c>
@@ -5279,7 +5279,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>203</v>
       </c>
@@ -5307,7 +5307,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>204</v>
       </c>
@@ -5335,7 +5335,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>205</v>
       </c>
@@ -5363,7 +5363,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>206</v>
       </c>
@@ -5391,7 +5391,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>207</v>
       </c>
@@ -5421,7 +5421,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>221</v>
       </c>
@@ -5449,7 +5449,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>209</v>
       </c>
@@ -5477,7 +5477,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>210</v>
       </c>
@@ -5507,7 +5507,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>212</v>
       </c>
@@ -5537,7 +5537,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>214</v>
       </c>
@@ -5565,7 +5565,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>216</v>
       </c>
@@ -5593,7 +5593,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="126" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>217</v>
       </c>
@@ -5621,7 +5621,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="127" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>218</v>
       </c>
@@ -5649,7 +5649,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="128" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>219</v>
       </c>
@@ -5677,7 +5677,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="129" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>220</v>
       </c>
@@ -5705,7 +5705,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="130" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>221</v>
       </c>
@@ -5733,7 +5733,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="131" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>222</v>
       </c>
@@ -5761,7 +5761,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="132" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>223</v>
       </c>
@@ -5791,7 +5791,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="133" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>224</v>
       </c>
@@ -5819,7 +5819,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="134" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>225</v>
       </c>
@@ -5847,7 +5847,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="135" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>226</v>
       </c>
@@ -5875,7 +5875,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="136" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>227</v>
       </c>
@@ -5903,7 +5903,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="137" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>228</v>
       </c>
@@ -5933,7 +5933,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="138" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>231</v>
       </c>
@@ -5961,7 +5961,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="139" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>232</v>
       </c>
@@ -5989,7 +5989,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="140" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>233</v>
       </c>
@@ -6017,7 +6017,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="141" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>234</v>
       </c>
@@ -6045,7 +6045,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="142" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
         <v>235</v>
       </c>
@@ -6073,7 +6073,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="143" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>236</v>
       </c>
@@ -6103,7 +6103,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="144" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
         <v>238</v>
       </c>
@@ -6131,7 +6131,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="145" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
         <v>239</v>
       </c>
@@ -6159,7 +6159,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="146" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>240</v>
       </c>
@@ -6189,7 +6189,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="147" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>242</v>
       </c>
@@ -6217,7 +6217,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="148" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A148" s="3" t="s">
         <v>243</v>
       </c>
@@ -6245,7 +6245,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="149" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A149" s="3" t="s">
         <v>245</v>
       </c>
@@ -6273,7 +6273,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="150" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A150" s="3" t="s">
         <v>246</v>
       </c>
@@ -6303,7 +6303,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="151" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
         <v>248</v>
       </c>
@@ -6331,7 +6331,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="152" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
         <v>250</v>
       </c>
@@ -6359,7 +6359,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="153" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
         <v>251</v>
       </c>
@@ -6387,7 +6387,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="154" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
         <v>252</v>
       </c>
@@ -6415,7 +6415,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="155" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
         <v>253</v>
       </c>
@@ -6443,7 +6443,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="156" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
         <v>254</v>
       </c>
@@ -6471,7 +6471,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="157" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
         <v>255</v>
       </c>
@@ -6499,7 +6499,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="158" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
         <v>257</v>
       </c>
@@ -6527,7 +6527,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="159" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
         <v>258</v>
       </c>
@@ -6555,7 +6555,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="160" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
         <v>259</v>
       </c>
@@ -6583,7 +6583,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="161" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
         <v>260</v>
       </c>
@@ -6611,7 +6611,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="162" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
         <v>261</v>
       </c>
@@ -6639,7 +6639,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="163" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
         <v>262</v>
       </c>
@@ -6667,7 +6667,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="164" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
         <v>263</v>
       </c>
@@ -6697,7 +6697,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="165" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A165" s="3" t="s">
         <v>264</v>
       </c>
@@ -6725,7 +6725,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="166" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A166" s="3" t="s">
         <v>266</v>
       </c>
@@ -6753,7 +6753,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="167" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A167" s="3" t="s">
         <v>267</v>
       </c>
@@ -6783,7 +6783,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="168" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A168" s="3" t="s">
         <v>270</v>
       </c>
@@ -6811,7 +6811,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="169" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A169" s="3" t="s">
         <v>272</v>
       </c>
@@ -6839,7 +6839,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="170" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A170" s="3" t="s">
         <v>274</v>
       </c>
@@ -6867,7 +6867,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="171" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
         <v>275</v>
       </c>
@@ -6897,7 +6897,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="172" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A172" s="3" t="s">
         <v>277</v>
       </c>
@@ -6925,7 +6925,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="173" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A173" s="3" t="s">
         <v>278</v>
       </c>
@@ -6955,7 +6955,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="174" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
         <v>279</v>
       </c>
@@ -6983,7 +6983,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="175" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
         <v>280</v>
       </c>
@@ -7011,7 +7011,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="176" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
         <v>281</v>
       </c>
@@ -7039,7 +7039,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="177" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
         <v>282</v>
       </c>
@@ -7067,7 +7067,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="178" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
         <v>283</v>
       </c>
@@ -7095,7 +7095,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="179" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
         <v>284</v>
       </c>
@@ -7123,7 +7123,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="180" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
         <v>285</v>
       </c>
@@ -7151,7 +7151,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="181" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
         <v>286</v>
       </c>
@@ -7179,7 +7179,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="182" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
         <v>287</v>
       </c>
@@ -7207,7 +7207,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="183" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
         <v>288</v>
       </c>
@@ -7235,7 +7235,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="184" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
         <v>289</v>
       </c>
@@ -7265,7 +7265,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="185" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
         <v>290</v>
       </c>
@@ -7295,7 +7295,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="186" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
         <v>292</v>
       </c>
@@ -7323,7 +7323,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="187" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
         <v>293</v>
       </c>
@@ -7353,7 +7353,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="188" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A188" s="3" t="s">
         <v>295</v>
       </c>
@@ -7381,7 +7381,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="189" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
         <v>296</v>
       </c>
@@ -7409,7 +7409,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="190" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
         <v>297</v>
       </c>
@@ -7437,7 +7437,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="191" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
         <v>298</v>
       </c>
@@ -7467,7 +7467,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="192" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
         <v>300</v>
       </c>
@@ -7497,7 +7497,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="193" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A193" s="3" t="s">
         <v>301</v>
       </c>
@@ -7525,7 +7525,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="194" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A194" s="3" t="s">
         <v>302</v>
       </c>
@@ -7553,7 +7553,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="195" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A195" s="3" t="s">
         <v>303</v>
       </c>
@@ -7581,7 +7581,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="196" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A196" s="3" t="s">
         <v>304</v>
       </c>
@@ -7609,7 +7609,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="197" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A197" s="3" t="s">
         <v>305</v>
       </c>
@@ -7637,7 +7637,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="198" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A198" s="3" t="s">
         <v>307</v>
       </c>
@@ -7665,7 +7665,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="199" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A199" s="3" t="s">
         <v>308</v>
       </c>
@@ -7693,7 +7693,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="200" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
         <v>309</v>
       </c>
@@ -7721,7 +7721,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="201" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
         <v>311</v>
       </c>
@@ -7749,7 +7749,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="202" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A202" s="3" t="s">
         <v>312</v>
       </c>
@@ -7777,7 +7777,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="203" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A203" s="3" t="s">
         <v>313</v>
       </c>
@@ -7805,7 +7805,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="204" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A204" s="3" t="s">
         <v>314</v>
       </c>
@@ -7833,7 +7833,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="205" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A205" s="3" t="s">
         <v>315</v>
       </c>
@@ -7863,7 +7863,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="206" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A206" s="3" t="s">
         <v>316</v>
       </c>
@@ -7891,7 +7891,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="207" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
         <v>317</v>
       </c>
@@ -7919,7 +7919,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="208" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
         <v>318</v>
       </c>
@@ -7947,7 +7947,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="209" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
         <v>319</v>
       </c>
@@ -7977,7 +7977,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="210" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
         <v>320</v>
       </c>
@@ -8007,7 +8007,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="211" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
         <v>322</v>
       </c>
@@ -8035,7 +8035,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="212" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
         <v>323</v>
       </c>
@@ -8065,7 +8065,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="213" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
         <v>324</v>
       </c>
@@ -8093,7 +8093,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="214" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
         <v>325</v>
       </c>
@@ -8121,7 +8121,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="215" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
         <v>327</v>
       </c>
@@ -8149,7 +8149,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="216" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A216" s="3" t="s">
         <v>328</v>
       </c>
@@ -8177,7 +8177,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="217" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A217" s="3" t="s">
         <v>329</v>
       </c>
@@ -8205,7 +8205,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="218" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A218" s="3" t="s">
         <v>330</v>
       </c>
@@ -8235,7 +8235,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="219" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A219" s="3" t="s">
         <v>331</v>
       </c>
@@ -8263,7 +8263,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="220" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A220" s="3" t="s">
         <v>332</v>
       </c>
@@ -8291,7 +8291,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="221" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
         <v>333</v>
       </c>
@@ -8319,7 +8319,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="222" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
         <v>334</v>
       </c>
@@ -8347,7 +8347,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="223" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
         <v>335</v>
       </c>
@@ -8377,7 +8377,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="224" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
         <v>336</v>
       </c>
@@ -8405,7 +8405,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="225" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
         <v>337</v>
       </c>
@@ -8435,7 +8435,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="226" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
         <v>338</v>
       </c>
@@ -8463,7 +8463,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="227" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
         <v>339</v>
       </c>
@@ -8491,7 +8491,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="228" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
         <v>340</v>
       </c>
@@ -8521,7 +8521,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="229" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
         <v>341</v>
       </c>
@@ -8549,7 +8549,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="230" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A230" t="s">
         <v>342</v>
       </c>
@@ -8577,7 +8577,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="231" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A231" t="s">
         <v>343</v>
       </c>
@@ -8605,7 +8605,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="232" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A232" t="s">
         <v>345</v>
       </c>
@@ -8633,7 +8633,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="233" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A233" t="s">
         <v>346</v>
       </c>
@@ -8661,7 +8661,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="234" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A234" t="s">
         <v>347</v>
       </c>
@@ -8689,7 +8689,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="235" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A235" t="s">
         <v>348</v>
       </c>
@@ -8717,7 +8717,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="236" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A236" t="s">
         <v>350</v>
       </c>
@@ -8745,7 +8745,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="237" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A237" t="s">
         <v>351</v>
       </c>
@@ -8773,7 +8773,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="238" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A238" s="3" t="s">
         <v>352</v>
       </c>
@@ -8801,7 +8801,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="239" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A239" s="3" t="s">
         <v>353</v>
       </c>
@@ -8829,7 +8829,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="240" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A240" s="3" t="s">
         <v>354</v>
       </c>
@@ -8857,7 +8857,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="241" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A241" s="3" t="s">
         <v>355</v>
       </c>
@@ -8885,7 +8885,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="242" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A242" s="3" t="s">
         <v>356</v>
       </c>
@@ -8913,7 +8913,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="243" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A243" s="3" t="s">
         <v>357</v>
       </c>
@@ -8941,7 +8941,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="244" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A244" s="3" t="s">
         <v>358</v>
       </c>
@@ -8969,7 +8969,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="245" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A245" s="3" t="s">
         <v>359</v>
       </c>
@@ -8997,7 +8997,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="246" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A246" t="s">
         <v>360</v>
       </c>
@@ -9025,7 +9025,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="247" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A247" t="s">
         <v>361</v>
       </c>
@@ -9055,7 +9055,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="248" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A248" s="3" t="s">
         <v>362</v>
       </c>
@@ -9085,7 +9085,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="249" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A249" t="s">
         <v>363</v>
       </c>
@@ -9113,7 +9113,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="250" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A250" t="s">
         <v>365</v>
       </c>
@@ -9141,7 +9141,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="251" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A251" t="s">
         <v>366</v>
       </c>
@@ -9171,7 +9171,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="252" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A252" t="s">
         <v>367</v>
       </c>
@@ -9201,7 +9201,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="253" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A253" t="s">
         <v>368</v>
       </c>
@@ -9231,7 +9231,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="254" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A254" t="s">
         <v>369</v>
       </c>
@@ -9259,7 +9259,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="255" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A255" t="s">
         <v>370</v>
       </c>
@@ -9287,7 +9287,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="256" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A256" t="s">
         <v>371</v>
       </c>
@@ -9317,7 +9317,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="257" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A257" t="s">
         <v>372</v>
       </c>
@@ -9345,7 +9345,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="258" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A258" t="s">
         <v>373</v>
       </c>
@@ -9373,7 +9373,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="259" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A259" t="s">
         <v>374</v>
       </c>
@@ -9401,7 +9401,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="260" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A260" t="s">
         <v>375</v>
       </c>
@@ -9429,7 +9429,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="261" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A261" t="s">
         <v>376</v>
       </c>
@@ -9457,7 +9457,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="262" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A262" t="s">
         <v>377</v>
       </c>
@@ -9485,7 +9485,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="263" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A263" t="s">
         <v>378</v>
       </c>
@@ -9513,7 +9513,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="264" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A264" t="s">
         <v>379</v>
       </c>
@@ -9543,7 +9543,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="265" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A265" t="s">
         <v>380</v>
       </c>
@@ -9571,7 +9571,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="266" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A266" t="s">
         <v>382</v>
       </c>
@@ -9599,7 +9599,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="267" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A267" t="s">
         <v>383</v>
       </c>
@@ -9627,7 +9627,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="268" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A268" t="s">
         <v>384</v>
       </c>
@@ -9655,7 +9655,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="269" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A269" t="s">
         <v>385</v>
       </c>
@@ -9683,7 +9683,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="270" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A270" t="s">
         <v>386</v>
       </c>
@@ -9713,7 +9713,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="271" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A271" t="s">
         <v>387</v>
       </c>
@@ -9741,7 +9741,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="272" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A272" t="s">
         <v>389</v>
       </c>
@@ -9769,7 +9769,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="273" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A273" t="s">
         <v>390</v>
       </c>
@@ -9797,7 +9797,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="274" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A274" s="3" t="s">
         <v>391</v>
       </c>
@@ -9827,7 +9827,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="275" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A275" s="3" t="s">
         <v>392</v>
       </c>
@@ -9855,7 +9855,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="276" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A276" s="3" t="s">
         <v>394</v>
       </c>
@@ -9883,7 +9883,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="277" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A277" s="3" t="s">
         <v>395</v>
       </c>
@@ -9911,7 +9911,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="278" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A278" t="s">
         <v>396</v>
       </c>
@@ -9939,7 +9939,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="279" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A279" t="s">
         <v>397</v>
       </c>
@@ -9967,7 +9967,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="280" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A280" t="s">
         <v>398</v>
       </c>
@@ -9995,7 +9995,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="281" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A281" t="s">
         <v>399</v>
       </c>
@@ -10023,7 +10023,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="282" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A282" t="s">
         <v>400</v>
       </c>
@@ -10051,7 +10051,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="283" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A283" t="s">
         <v>401</v>
       </c>
@@ -10079,7 +10079,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="284" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A284" t="s">
         <v>402</v>
       </c>
@@ -10109,7 +10109,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="285" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A285" t="s">
         <v>403</v>
       </c>
@@ -10137,7 +10137,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="286" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A286" t="s">
         <v>404</v>
       </c>
@@ -10165,7 +10165,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="287" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A287" t="s">
         <v>405</v>
       </c>
@@ -10193,7 +10193,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="288" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A288" t="s">
         <v>406</v>
       </c>
@@ -10223,7 +10223,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="289" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A289" s="3" t="s">
         <v>407</v>
       </c>
@@ -10251,7 +10251,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="290" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A290" s="3" t="s">
         <v>408</v>
       </c>
@@ -10279,7 +10279,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="291" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A291" s="3" t="s">
         <v>409</v>
       </c>
@@ -10307,7 +10307,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="292" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A292" t="s">
         <v>410</v>
       </c>
@@ -10335,7 +10335,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="293" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A293" t="s">
         <v>414</v>
       </c>
@@ -10363,7 +10363,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="294" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A294" t="s">
         <v>415</v>
       </c>
@@ -10393,7 +10393,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="295" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A295" t="s">
         <v>416</v>
       </c>
@@ -10421,7 +10421,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="296" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A296" t="s">
         <v>417</v>
       </c>
@@ -10451,7 +10451,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="297" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A297" t="s">
         <v>418</v>
       </c>
@@ -10479,7 +10479,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="298" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A298" t="s">
         <v>419</v>
       </c>
@@ -10509,7 +10509,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="299" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A299" t="s">
         <v>420</v>
       </c>
@@ -10539,7 +10539,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="300" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A300" t="s">
         <v>421</v>
       </c>
@@ -10569,7 +10569,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="301" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A301" t="s">
         <v>422</v>
       </c>
@@ -10597,7 +10597,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="302" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A302" t="s">
         <v>423</v>
       </c>
@@ -10625,7 +10625,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="303" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A303" t="s">
         <v>424</v>
       </c>
@@ -10653,7 +10653,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="304" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A304" t="s">
         <v>426</v>
       </c>
@@ -10681,7 +10681,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="305" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A305" t="s">
         <v>428</v>
       </c>
@@ -10709,7 +10709,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="306" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A306" t="s">
         <v>429</v>
       </c>
@@ -10737,7 +10737,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="307" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A307" s="3" t="s">
         <v>430</v>
       </c>
@@ -10765,7 +10765,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="308" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A308" s="3" t="s">
         <v>431</v>
       </c>
@@ -10793,7 +10793,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="309" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A309" s="3" t="s">
         <v>432</v>
       </c>
@@ -10821,7 +10821,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="310" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A310" t="s">
         <v>433</v>
       </c>
@@ -10851,7 +10851,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="311" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A311" t="s">
         <v>434</v>
       </c>
@@ -10879,7 +10879,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="312" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A312" t="s">
         <v>435</v>
       </c>
@@ -10907,7 +10907,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="313" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A313" s="3" t="s">
         <v>436</v>
       </c>
@@ -10935,7 +10935,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="314" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A314" s="3" t="s">
         <v>438</v>
       </c>
@@ -10965,7 +10965,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="315" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A315" s="3" t="s">
         <v>439</v>
       </c>
@@ -10995,7 +10995,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="316" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A316" t="s">
         <v>440</v>
       </c>
@@ -11023,7 +11023,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="317" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A317" t="s">
         <v>442</v>
       </c>
@@ -11051,7 +11051,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="318" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A318" t="s">
         <v>443</v>
       </c>
@@ -11079,7 +11079,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="319" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A319" t="s">
         <v>444</v>
       </c>
@@ -11107,7 +11107,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="320" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A320" t="s">
         <v>445</v>
       </c>
@@ -11135,7 +11135,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="321" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A321" t="s">
         <v>446</v>
       </c>
@@ -11163,7 +11163,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="322" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A322" t="s">
         <v>447</v>
       </c>
@@ -11191,7 +11191,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="323" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A323" t="s">
         <v>448</v>
       </c>
@@ -11219,7 +11219,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="324" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A324" t="s">
         <v>449</v>
       </c>
@@ -11247,7 +11247,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="325" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A325" t="s">
         <v>450</v>
       </c>
@@ -11275,7 +11275,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="326" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A326" t="s">
         <v>451</v>
       </c>
@@ -11303,7 +11303,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="327" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A327" t="s">
         <v>452</v>
       </c>
@@ -11333,7 +11333,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="328" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A328" t="s">
         <v>453</v>
       </c>
@@ -11361,7 +11361,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="329" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A329" t="s">
         <v>454</v>
       </c>
@@ -11389,7 +11389,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="330" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A330" t="s">
         <v>455</v>
       </c>
@@ -11417,7 +11417,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="331" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A331" t="s">
         <v>456</v>
       </c>
@@ -11445,7 +11445,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="332" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A332" t="s">
         <v>457</v>
       </c>
@@ -11473,7 +11473,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="333" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A333" t="s">
         <v>458</v>
       </c>
@@ -11501,7 +11501,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="334" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A334" t="s">
         <v>459</v>
       </c>
@@ -11531,7 +11531,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="335" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A335" t="s">
         <v>460</v>
       </c>
@@ -11559,7 +11559,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="336" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A336" t="s">
         <v>461</v>
       </c>
@@ -11589,7 +11589,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="337" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A337" t="s">
         <v>462</v>
       </c>
@@ -11617,7 +11617,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="338" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A338" t="s">
         <v>463</v>
       </c>
@@ -11647,7 +11647,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="339" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A339" t="s">
         <v>464</v>
       </c>
@@ -11675,7 +11675,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="340" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A340" t="s">
         <v>465</v>
       </c>
@@ -11703,7 +11703,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="341" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A341" s="3" t="s">
         <v>466</v>
       </c>
@@ -11731,7 +11731,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="342" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A342" s="3" t="s">
         <v>467</v>
       </c>
@@ -11759,7 +11759,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="343" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A343" s="3" t="s">
         <v>468</v>
       </c>
@@ -11787,7 +11787,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="344" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A344" t="s">
         <v>469</v>
       </c>
@@ -11815,7 +11815,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="345" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A345" t="s">
         <v>470</v>
       </c>
@@ -11843,7 +11843,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="346" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A346" s="3" t="s">
         <v>471</v>
       </c>
@@ -11871,7 +11871,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="347" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A347" s="3" t="s">
         <v>472</v>
       </c>
@@ -11899,7 +11899,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="348" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A348" s="3" t="s">
         <v>473</v>
       </c>
@@ -11927,7 +11927,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="349" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A349" t="s">
         <v>474</v>
       </c>
@@ -11959,7 +11959,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="350" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A350" t="s">
         <v>475</v>
       </c>
@@ -11987,7 +11987,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="351" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A351" t="s">
         <v>476</v>
       </c>
@@ -12015,7 +12015,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="352" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A352" t="s">
         <v>477</v>
       </c>
@@ -12043,7 +12043,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="353" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A353" t="s">
         <v>478</v>
       </c>
@@ -12071,7 +12071,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="354" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A354" t="s">
         <v>479</v>
       </c>
@@ -12099,7 +12099,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="355" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A355" t="s">
         <v>480</v>
       </c>
@@ -12127,7 +12127,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="356" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A356" t="s">
         <v>481</v>
       </c>
@@ -12155,7 +12155,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="357" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A357" t="s">
         <v>482</v>
       </c>
@@ -12183,7 +12183,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="358" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A358" t="s">
         <v>483</v>
       </c>
@@ -12211,7 +12211,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="359" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A359" t="s">
         <v>484</v>
       </c>
@@ -12239,7 +12239,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="360" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A360" t="s">
         <v>485</v>
       </c>
@@ -12267,7 +12267,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="361" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A361" t="s">
         <v>486</v>
       </c>
@@ -12295,7 +12295,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="362" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A362" t="s">
         <v>487</v>
       </c>
@@ -12325,7 +12325,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="363" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A363" t="s">
         <v>488</v>
       </c>
@@ -12353,7 +12353,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="364" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A364" t="s">
         <v>489</v>
       </c>
@@ -12381,7 +12381,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="365" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A365" t="s">
         <v>490</v>
       </c>
@@ -12409,7 +12409,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="366" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A366" t="s">
         <v>492</v>
       </c>
@@ -12439,7 +12439,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="367" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A367" t="s">
         <v>494</v>
       </c>
@@ -12467,7 +12467,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="368" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A368" t="s">
         <v>495</v>
       </c>
@@ -12495,7 +12495,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="369" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A369" t="s">
         <v>497</v>
       </c>
@@ -12523,7 +12523,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="370" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A370" s="3" t="s">
         <v>498</v>
       </c>
@@ -12551,7 +12551,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="371" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A371" s="3" t="s">
         <v>499</v>
       </c>
@@ -12579,7 +12579,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="372" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A372" s="3" t="s">
         <v>500</v>
       </c>
@@ -12607,7 +12607,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="373" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A373" t="s">
         <v>501</v>
       </c>
@@ -12635,7 +12635,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="374" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A374" t="s">
         <v>502</v>
       </c>
@@ -12663,7 +12663,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="375" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A375" s="3" t="s">
         <v>503</v>
       </c>
@@ -12693,7 +12693,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="376" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A376" s="3" t="s">
         <v>504</v>
       </c>
@@ -12723,7 +12723,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="377" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A377" s="3" t="s">
         <v>505</v>
       </c>
@@ -12751,7 +12751,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="378" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A378" s="3" t="s">
         <v>506</v>
       </c>
@@ -12779,7 +12779,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="379" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A379" s="3" t="s">
         <v>507</v>
       </c>
@@ -12807,7 +12807,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="380" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A380" s="3" t="s">
         <v>508</v>
       </c>
@@ -12835,7 +12835,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="381" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A381" t="s">
         <v>509</v>
       </c>
@@ -12863,7 +12863,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="382" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A382" t="s">
         <v>510</v>
       </c>
@@ -12891,7 +12891,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="383" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="383" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A383" t="s">
         <v>511</v>
       </c>
@@ -12919,7 +12919,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="384" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="384" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A384" t="s">
         <v>512</v>
       </c>
@@ -12947,7 +12947,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="385" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A385" t="s">
         <v>513</v>
       </c>
@@ -12975,7 +12975,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="386" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="386" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A386" t="s">
         <v>514</v>
       </c>
@@ -13003,7 +13003,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="387" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="387" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A387" t="s">
         <v>515</v>
       </c>
@@ -13033,7 +13033,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="388" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="388" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A388" t="s">
         <v>516</v>
       </c>
@@ -13061,7 +13061,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="389" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="389" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A389" t="s">
         <v>517</v>
       </c>
@@ -13089,7 +13089,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="390" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="390" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A390" t="s">
         <v>518</v>
       </c>
@@ -13117,7 +13117,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="391" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="391" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A391" s="3" t="s">
         <v>519</v>
       </c>
@@ -13145,7 +13145,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="392" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="392" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A392" s="3" t="s">
         <v>520</v>
       </c>
@@ -13173,7 +13173,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="393" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="393" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A393" t="s">
         <v>521</v>
       </c>
@@ -13201,7 +13201,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="394" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="394" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A394" t="s">
         <v>522</v>
       </c>
@@ -13231,7 +13231,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="395" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="395" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A395" t="s">
         <v>524</v>
       </c>
@@ -13259,7 +13259,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="396" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="396" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A396" t="s">
         <v>525</v>
       </c>
@@ -13287,7 +13287,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="397" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="397" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A397" t="s">
         <v>526</v>
       </c>
@@ -13317,7 +13317,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="398" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="398" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A398" s="3" t="s">
         <v>527</v>
       </c>
@@ -13345,7 +13345,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="399" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="399" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A399" s="3" t="s">
         <v>528</v>
       </c>

</xml_diff>